<commit_message>
added get_data(column_name) in utils.py successfully tested getting the value by column name
heading & corresponding values are stored in the dictionary for the row number provided.
</commit_message>
<xml_diff>
--- a/POMFramework_POC/TestData/TDexcel.xlsx
+++ b/POMFramework_POC/TestData/TDexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sindh\PycharmProjects\POMFramework_POC\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22725942-2075-42BB-AE48-C8EDA26EB7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72BC103-21A1-4CCE-97B5-C7031264BF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13605" yWindow="2430" windowWidth="11925" windowHeight="8370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,135 +396,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>100036589</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>100036590</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>100036591</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>100036592</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>100036593</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>100036594</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modularization of get_data() to read from excel. get_data() is generic.  Wrkbk & sheet values are imported from Config.
New URL skillboard - In-progress
</commit_message>
<xml_diff>
--- a/POMFramework_POC/TestData/TDexcel.xlsx
+++ b/POMFramework_POC/TestData/TDexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sindh\PycharmProjects\POMFramework_POC\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72BC103-21A1-4CCE-97B5-C7031264BF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF893EB-4A58-48FA-9F3A-4203245FDF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>Region</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>tc_6</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>sindhu</t>
+  </si>
+  <si>
+    <t>boston</t>
   </si>
 </sst>
 </file>
@@ -394,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F3" sqref="F3:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,7 +418,7 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -422,8 +434,14 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -439,8 +457,14 @@
       <c r="E2" s="1">
         <v>100036589</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -456,8 +480,14 @@
       <c r="E3" s="1">
         <v>100036590</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -473,8 +503,14 @@
       <c r="E4" s="1">
         <v>100036591</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -490,8 +526,14 @@
       <c r="E5" s="1">
         <v>100036592</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -507,8 +549,14 @@
       <c r="E6" s="1">
         <v>100036593</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -523,6 +571,12 @@
       </c>
       <c r="E7" s="1">
         <v>100036594</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>